<commit_message>
dodanie strony drugiej opisującej montaż i instalację oraz numery stron
</commit_message>
<xml_diff>
--- a/kosztorys-wstepny.xlsx
+++ b/kosztorys-wstepny.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Arkusz1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Arkusz2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Wrocław, 15.01.2025r.</t>
   </si>
@@ -56,12 +57,72 @@
   <si>
     <t>Podpis sporządzającego:</t>
   </si>
+  <si>
+    <t>Montaż i instalacja lokalnej sieci komputerowej
+ w budynku przy ulicy Zielonej w Warszawie</t>
+  </si>
+  <si>
+    <t>1.1 Podstawa sporządzenia kosztorysu:</t>
+  </si>
+  <si>
+    <t>- Specyfikacja projektu sieci lokalnej,</t>
+  </si>
+  <si>
+    <t>- Wizja lokalna,</t>
+  </si>
+  <si>
+    <t>1.2 Zakres prac:</t>
+  </si>
+  <si>
+    <t>- Instalacja korytek kablowych dla okablowania poziomego w przestrzeni sufitu podwieszanego,</t>
+  </si>
+  <si>
+    <t>- Instalacja okablowania poziomego - przewód F/UTP w kategorii 6. Przewody są prowadzone w przestrzeni sufitu podwieszanego,</t>
+  </si>
+  <si>
+    <t>- Instalacja gniazd abonenckich, zgodnie z normą TIA/EIA 568B na wysokości 25 cm od podłogi,</t>
+  </si>
+  <si>
+    <t>- Montaż szafy dystrybucyjnej typu rack w rejestracji, wiszącej, w rozmiarze 12U.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Przedmiar prac</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Tabela 1.1</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Długości przewodów, które zostaną użyte do stworzenia lokalnej sieci komputerowej</t>
+    </r>
+  </si>
+  <si>
+    <t>Połączenie z ... do ...</t>
+  </si>
+  <si>
+    <t>Długość korytek (m)</t>
+  </si>
+  <si>
+    <t>Długość przewodów (m)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -117,7 +178,20 @@
       <name val="Liberation Sans"/>
     </font>
     <font>
-      <sz val="18.0"/>
+      <b/>
+      <sz val="21.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FFC9211E"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
       <color rgb="FFC9211E"/>
       <name val="Liberation Sans"/>
     </font>
@@ -142,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -180,23 +254,41 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -207,6 +299,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -408,9 +504,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
@@ -419,105 +516,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="179.25" customHeight="1">
+    <row r="3">
       <c r="E3" s="2"/>
     </row>
     <row r="4">
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="E5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10">
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18">
-      <c r="D18" s="6"/>
-      <c r="E18" s="11"/>
-    </row>
     <row r="19">
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
-    </row>
-    <row r="22" ht="159.0" customHeight="1">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -528,9 +593,8 @@
       <c r="H22" s="6"/>
     </row>
     <row r="23">
-      <c r="A23" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
@@ -539,79 +603,45 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="A24" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="E24" s="9" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="8"/>
+      <c r="A25" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" ht="41.25" customHeight="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27">
       <c r="D27" s="6"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
     </row>
     <row r="28">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="E28" s="7"/>
     </row>
     <row r="29">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
     </row>
     <row r="30">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31">
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" ht="159.0" customHeight="1">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -622,11 +652,12 @@
       <c r="H31" s="6"/>
     </row>
     <row r="32">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
+      <c r="A32" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="11"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -642,9 +673,10 @@
       <c r="H33" s="6"/>
     </row>
     <row r="34">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+      <c r="A34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="8"/>
       <c r="D34" s="6"/>
       <c r="E34" s="11"/>
       <c r="F34" s="6"/>
@@ -652,8 +684,9 @@
       <c r="H34" s="6"/>
     </row>
     <row r="35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
+      <c r="A35" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="7"/>
@@ -661,105 +694,574 @@
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
     </row>
-    <row r="36">
-      <c r="E36" s="12"/>
+    <row r="36" ht="41.25" customHeight="1">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37">
-      <c r="E37" s="13"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="38">
-      <c r="E38" s="14"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
     <row r="39">
-      <c r="E39" s="13"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
     </row>
     <row r="40">
-      <c r="E40" s="14"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41">
-      <c r="E41" s="13"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42">
-      <c r="E42" s="14"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43">
-      <c r="E43" s="13"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="10">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="E44" s="14"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45">
-      <c r="E45" s="13"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46">
-      <c r="E46" s="14"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47">
-      <c r="E47" s="13"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48">
-      <c r="E48" s="14"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="10"/>
     </row>
     <row r="49">
-      <c r="E49" s="13"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="10"/>
     </row>
     <row r="50">
-      <c r="E50" s="13"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="10"/>
     </row>
     <row r="51">
-      <c r="E51" s="13"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="10"/>
     </row>
     <row r="52">
-      <c r="E52" s="13"/>
+      <c r="E52" s="12"/>
     </row>
     <row r="53">
-      <c r="E53" s="13"/>
-    </row>
-    <row r="54">
-      <c r="E54" s="15"/>
-    </row>
-    <row r="55">
-      <c r="E55" s="16"/>
-    </row>
-    <row r="56">
-      <c r="E56" s="16"/>
+      <c r="A53" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="57">
-      <c r="E57" s="17"/>
+      <c r="E57" s="14"/>
     </row>
     <row r="58">
-      <c r="E58" s="18"/>
+      <c r="E58" s="14"/>
     </row>
     <row r="59">
-      <c r="E59" s="18"/>
+      <c r="E59" s="15"/>
     </row>
     <row r="60">
-      <c r="E60" s="17"/>
+      <c r="E60" s="15"/>
     </row>
     <row r="61">
-      <c r="E61" s="18"/>
+      <c r="E61" s="15"/>
     </row>
     <row r="62">
-      <c r="E62" s="18"/>
+      <c r="E62" s="15"/>
     </row>
     <row r="63">
-      <c r="E63" s="18"/>
+      <c r="E63" s="15"/>
     </row>
     <row r="64">
-      <c r="E64" s="18"/>
+      <c r="E64" s="15"/>
+    </row>
+    <row r="65">
+      <c r="E65" s="14"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="6"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="6"/>
+      <c r="B68" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="6"/>
+      <c r="B69" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="6"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="6"/>
+      <c r="B73" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="6"/>
+      <c r="B74" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="6"/>
+      <c r="B76" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="6"/>
+      <c r="B77" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="6"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="6"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90">
+      <c r="E90" s="23"/>
+    </row>
+    <row r="98">
+      <c r="H98" s="24">
+        <v>2.0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="F16:H21"/>
-    <mergeCell ref="A16:C21"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="A6:H9"/>
+  <mergeCells count="13">
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="A15:H18"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="A25:C30"/>
+    <mergeCell ref="F25:H30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A53:H56"/>
+    <mergeCell ref="B73:H73"/>
+    <mergeCell ref="B74:H75"/>
+  </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="9">
+      <c r="F9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17">
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18">
+      <c r="F18" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="F24" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="F26" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="F18:M21"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
dodanie rozdziału przedmiary prac, stworzenie tabelki długości przewodów
</commit_message>
<xml_diff>
--- a/kosztorys-wstepny.xlsx
+++ b/kosztorys-wstepny.xlsx
@@ -4,7 +4,6 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Arkusz1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Arkusz2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Wrocław, 15.01.2025r.</t>
   </si>
@@ -86,9 +85,6 @@
     <t>- Montaż szafy dystrybucyjnej typu rack w rejestracji, wiszącej, w rozmiarze 12U.</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>Przedmiar prac</t>
   </si>
   <si>
@@ -97,6 +93,7 @@
         <rFont val="Arial"/>
         <b/>
         <color theme="1"/>
+        <sz val="12.0"/>
       </rPr>
       <t>Tabela 1.1</t>
     </r>
@@ -104,6 +101,7 @@
       <rPr>
         <rFont val="Arial"/>
         <color theme="1"/>
+        <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve"> Długości przewodów, które zostaną użyte do stworzenia lokalnej sieci komputerowej</t>
     </r>
@@ -116,13 +114,40 @@
   </si>
   <si>
     <t>Długość przewodów (m)</t>
+  </si>
+  <si>
+    <t>Szafa rack - rejestracja</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 1</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 2</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 3</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 4</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 5</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 6</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 7</t>
+  </si>
+  <si>
+    <t>Razem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -201,22 +226,80 @@
       <color rgb="FFC9211E"/>
       <name val="Liberation Sans"/>
     </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font/>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666666"/>
+        <bgColor rgb="FF666666"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -289,6 +372,31 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -299,10 +407,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1117,8 +1221,779 @@
         <v>2.0</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" s="10"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="6"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="6"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="10"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="6"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="10"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="10"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="10"/>
+    </row>
+    <row r="107">
+      <c r="E107" s="12"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="6"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+    </row>
+    <row r="116">
+      <c r="C116" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D116" s="26"/>
+      <c r="E116" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F116" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H116" s="6"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="6"/>
+      <c r="C117" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D117" s="26"/>
+      <c r="E117" s="29">
+        <v>4.0</v>
+      </c>
+      <c r="F117" s="29">
+        <v>6.0</v>
+      </c>
+      <c r="H117" s="6"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="6"/>
+      <c r="C118" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D118" s="26"/>
+      <c r="E118" s="31">
+        <v>9.0</v>
+      </c>
+      <c r="F118" s="31">
+        <v>11.0</v>
+      </c>
+      <c r="H118" s="6"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="6"/>
+      <c r="C119" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D119" s="26"/>
+      <c r="E119" s="29">
+        <v>9.0</v>
+      </c>
+      <c r="F119" s="29">
+        <v>16.0</v>
+      </c>
+      <c r="H119" s="6"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="6"/>
+      <c r="C120" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D120" s="26"/>
+      <c r="E120" s="31">
+        <v>9.0</v>
+      </c>
+      <c r="F120" s="31">
+        <v>21.0</v>
+      </c>
+      <c r="H120" s="6"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="6"/>
+      <c r="C121" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D121" s="26"/>
+      <c r="E121" s="29">
+        <v>10.0</v>
+      </c>
+      <c r="F121" s="29">
+        <v>12.0</v>
+      </c>
+      <c r="H121" s="6"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="6"/>
+      <c r="C122" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D122" s="26"/>
+      <c r="E122" s="31">
+        <v>4.0</v>
+      </c>
+      <c r="F122" s="31">
+        <v>8.0</v>
+      </c>
+      <c r="H122" s="6"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="6"/>
+      <c r="C123" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D123" s="26"/>
+      <c r="E123" s="29">
+        <v>9.0</v>
+      </c>
+      <c r="F123" s="29">
+        <v>13.0</v>
+      </c>
+      <c r="H123" s="6"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="6"/>
+      <c r="C124" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D124" s="26"/>
+      <c r="E124" s="31">
+        <v>9.0</v>
+      </c>
+      <c r="F124" s="31">
+        <v>18.0</v>
+      </c>
+      <c r="H124" s="6"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="6"/>
+      <c r="C125" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D125" s="26"/>
+      <c r="E125" s="32">
+        <f t="shared" ref="E125:F125" si="1">sum(E117:E124)</f>
+        <v>63</v>
+      </c>
+      <c r="F125" s="32">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="H125" s="6"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="6"/>
+      <c r="B126" s="33"/>
+      <c r="C126" s="33"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="6"/>
+      <c r="B127" s="33"/>
+      <c r="C127" s="33"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="6"/>
+      <c r="B128" s="33"/>
+      <c r="C128" s="33"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="6"/>
+      <c r="B129" s="33"/>
+      <c r="C129" s="33"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="6"/>
+      <c r="B130" s="33"/>
+      <c r="C130" s="33"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="6"/>
+      <c r="B131" s="33"/>
+      <c r="C131" s="33"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="6"/>
+      <c r="B132" s="33"/>
+      <c r="C132" s="33"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
+      <c r="H132" s="6"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="6"/>
+      <c r="B133" s="33"/>
+      <c r="C133" s="33"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="6"/>
+      <c r="B134" s="33"/>
+      <c r="C134" s="33"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="6"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="6"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="6"/>
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="6"/>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="6"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="6"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="6"/>
+      <c r="F137" s="6"/>
+      <c r="G137" s="6"/>
+      <c r="H137" s="6"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="6"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="6"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="6"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="6"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="6"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+      <c r="F140" s="6"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="6"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+      <c r="F141" s="6"/>
+      <c r="G141" s="6"/>
+      <c r="H141" s="6"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="6"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="6"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="6"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="6"/>
+      <c r="F144" s="6"/>
+      <c r="G144" s="6"/>
+      <c r="H144" s="6"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="6"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="6"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="6"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6"/>
+      <c r="G146" s="6"/>
+      <c r="H146" s="6"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="6"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="6"/>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="6"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="6"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+      <c r="E148" s="6"/>
+      <c r="F148" s="6"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="6"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="6"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
+      <c r="E149" s="6"/>
+      <c r="F149" s="6"/>
+      <c r="G149" s="6"/>
+      <c r="H149" s="6"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="6"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="6"/>
+      <c r="F150" s="6"/>
+      <c r="G150" s="6"/>
+      <c r="H150" s="6"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="6"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="6"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="6"/>
+      <c r="F152" s="6"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="6"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="6"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
+      <c r="E153" s="6"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="6"/>
+      <c r="H153" s="6"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="6"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="6"/>
+      <c r="H154" s="6"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="6"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="E155" s="6"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="6"/>
+      <c r="H155" s="6"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="6"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+      <c r="E156" s="6"/>
+      <c r="F156" s="6"/>
+      <c r="G156" s="6"/>
+      <c r="H156" s="6"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="6"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+      <c r="E157" s="6"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="6"/>
+      <c r="H157" s="6"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="6"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="6"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="6"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="6"/>
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="6"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="6"/>
+      <c r="B165" s="6"/>
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
+      <c r="E165" s="6"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="6"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="6"/>
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+      <c r="E166" s="6"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="6"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="6"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
+      <c r="E167" s="6"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="6"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="6"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
+      <c r="E168" s="6"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="6"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="6"/>
+      <c r="G169" s="6"/>
+      <c r="H169" s="6"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="6"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
+      <c r="E170" s="6"/>
+      <c r="F170" s="6"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="6"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="6"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="6"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
+      <c r="E172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6"/>
+      <c r="H172" s="6"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="6"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+      <c r="E173" s="6"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="6"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="6"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
+      <c r="E175" s="6"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="6"/>
+      <c r="H175" s="6"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="6"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+      <c r="E176" s="6"/>
+      <c r="F176" s="6"/>
+      <c r="G176" s="6"/>
+      <c r="H176" s="6"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="6"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6"/>
+      <c r="H177" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="24">
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="A15:H18"/>
     <mergeCell ref="A24:C24"/>
@@ -1132,137 +2007,21 @@
     <mergeCell ref="A53:H56"/>
     <mergeCell ref="B73:H73"/>
     <mergeCell ref="B74:H75"/>
+    <mergeCell ref="A108:H111"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="9">
-      <c r="F9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10">
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12">
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13">
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="10"/>
-    </row>
-    <row r="14">
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="10"/>
-    </row>
-    <row r="15">
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16">
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17">
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18">
-      <c r="F18" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="F24" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="F26" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="F18:M21"/>
-  </mergeCells>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
dodanie tabeli przedmiaru prac, bez roboczogodzin
</commit_message>
<xml_diff>
--- a/kosztorys-wstepny.xlsx
+++ b/kosztorys-wstepny.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Wrocław, 15.01.2025r.</t>
   </si>
@@ -85,62 +85,90 @@
     <t>- Montaż szafy dystrybucyjnej typu rack w rejestracji, wiszącej, w rozmiarze 12U.</t>
   </si>
   <si>
+    <t>Długości przewodów, które zostaną użyte
+ do stworzenia lokalnej sieci komputerowej</t>
+  </si>
+  <si>
+    <t>Połączenie z ... do ...</t>
+  </si>
+  <si>
+    <t>Długość korytek (m)</t>
+  </si>
+  <si>
+    <t>Długość przewodów (m)</t>
+  </si>
+  <si>
+    <t>Szafa rack - rejestracja</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 1</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 2</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 3</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 4</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 5</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 6</t>
+  </si>
+  <si>
+    <t>Rejestracja - gabinet nr 7</t>
+  </si>
+  <si>
+    <t>Razem</t>
+  </si>
+  <si>
     <t>Przedmiar prac</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t>Tabela 1.1</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t xml:space="preserve"> Długości przewodów, które zostaną użyte do stworzenia lokalnej sieci komputerowej</t>
-    </r>
-  </si>
-  <si>
-    <t>Połączenie z ... do ...</t>
-  </si>
-  <si>
-    <t>Długość korytek (m)</t>
-  </si>
-  <si>
-    <t>Długość przewodów (m)</t>
-  </si>
-  <si>
-    <t>Szafa rack - rejestracja</t>
-  </si>
-  <si>
-    <t>Rejestracja - gabinet nr 1</t>
-  </si>
-  <si>
-    <t>Rejestracja - gabinet nr 2</t>
-  </si>
-  <si>
-    <t>Rejestracja - gabinet nr 3</t>
-  </si>
-  <si>
-    <t>Rejestracja - gabinet nr 4</t>
-  </si>
-  <si>
-    <t>Rejestracja - gabinet nr 5</t>
-  </si>
-  <si>
-    <t>Rejestracja - gabinet nr 6</t>
-  </si>
-  <si>
-    <t>Rejestracja - gabinet nr 7</t>
-  </si>
-  <si>
-    <t>Razem</t>
+    <t>Nazwa</t>
+  </si>
+  <si>
+    <t>Jednostka miary</t>
+  </si>
+  <si>
+    <t>Liczba</t>
+  </si>
+  <si>
+    <t>Roboczo-
+godziny</t>
+  </si>
+  <si>
+    <t>Montaż szafy dystrybucyjnej wiszącej</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Układanie korytek kablowych</t>
+  </si>
+  <si>
+    <t>metr</t>
+  </si>
+  <si>
+    <t>Montaż podwójnych gniazd abonenckich</t>
+  </si>
+  <si>
+    <t>sztuka</t>
+  </si>
+  <si>
+    <t>Instalacja okablowania w patchpanelu oraz odpowiednie oznakowanie</t>
+  </si>
+  <si>
+    <t>Montaż patchpaneli, organizerów przewodów oraz listew zasilającyh w szafie typu rack</t>
+  </si>
+  <si>
+    <t>Porządkowanie instalacji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Razem:  </t>
   </si>
 </sst>
 </file>
@@ -260,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -295,11 +323,22 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -381,23 +420,46 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -611,7 +673,7 @@
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
@@ -1246,236 +1308,218 @@
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
-      <c r="E101" s="7"/>
+      <c r="E101" s="11"/>
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
-      <c r="H101" s="6"/>
+      <c r="H101" s="10"/>
     </row>
     <row r="102">
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
-      <c r="E102" s="7"/>
+      <c r="E102" s="11"/>
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
-      <c r="H102" s="6"/>
+      <c r="H102" s="10"/>
     </row>
     <row r="103">
-      <c r="A103" s="6"/>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-      <c r="H103" s="10"/>
+      <c r="E103" s="12"/>
     </row>
     <row r="104">
-      <c r="A104" s="6"/>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="6"/>
-      <c r="H104" s="10"/>
-    </row>
-    <row r="105">
-      <c r="A105" s="6"/>
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="10"/>
-    </row>
-    <row r="106">
-      <c r="A106" s="6"/>
-      <c r="B106" s="6"/>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="6"/>
-      <c r="G106" s="6"/>
-      <c r="H106" s="10"/>
-    </row>
-    <row r="107">
-      <c r="E107" s="12"/>
+      <c r="A104" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="108">
-      <c r="A108" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="A108" s="10"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="6"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+    </row>
+    <row r="110">
+      <c r="C110" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" s="26"/>
+      <c r="E110" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F110" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H110" s="6"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="6"/>
+      <c r="C111" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D111" s="26"/>
+      <c r="E111" s="29">
+        <v>4.0</v>
+      </c>
+      <c r="F111" s="29">
+        <v>6.0</v>
+      </c>
+      <c r="H111" s="6"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="6"/>
+      <c r="C112" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" s="26"/>
+      <c r="E112" s="31">
+        <v>9.0</v>
+      </c>
+      <c r="F112" s="31">
+        <v>11.0</v>
+      </c>
+      <c r="H112" s="6"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="6"/>
+      <c r="C113" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D113" s="26"/>
+      <c r="E113" s="29">
+        <v>9.0</v>
+      </c>
+      <c r="F113" s="29">
+        <v>16.0</v>
+      </c>
+      <c r="H113" s="6"/>
     </row>
     <row r="114">
-      <c r="A114" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B114" s="6"/>
-      <c r="C114" s="6"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="6"/>
-      <c r="F114" s="6"/>
-      <c r="G114" s="6"/>
+      <c r="A114" s="6"/>
+      <c r="C114" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D114" s="26"/>
+      <c r="E114" s="31">
+        <v>9.0</v>
+      </c>
+      <c r="F114" s="31">
+        <v>21.0</v>
+      </c>
       <c r="H114" s="6"/>
     </row>
     <row r="115">
       <c r="A115" s="6"/>
-      <c r="B115" s="6"/>
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="6"/>
-      <c r="F115" s="6"/>
-      <c r="G115" s="6"/>
+      <c r="C115" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" s="26"/>
+      <c r="E115" s="29">
+        <v>10.0</v>
+      </c>
+      <c r="F115" s="29">
+        <v>12.0</v>
+      </c>
       <c r="H115" s="6"/>
     </row>
     <row r="116">
-      <c r="C116" s="25" t="s">
-        <v>22</v>
+      <c r="A116" s="6"/>
+      <c r="C116" s="30" t="s">
+        <v>29</v>
       </c>
       <c r="D116" s="26"/>
-      <c r="E116" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F116" s="27" t="s">
-        <v>24</v>
+      <c r="E116" s="31">
+        <v>4.0</v>
+      </c>
+      <c r="F116" s="31">
+        <v>8.0</v>
       </c>
       <c r="H116" s="6"/>
     </row>
     <row r="117">
       <c r="A117" s="6"/>
       <c r="C117" s="28" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D117" s="26"/>
       <c r="E117" s="29">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="F117" s="29">
-        <v>6.0</v>
+        <v>13.0</v>
       </c>
       <c r="H117" s="6"/>
     </row>
     <row r="118">
       <c r="A118" s="6"/>
       <c r="C118" s="30" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D118" s="26"/>
       <c r="E118" s="31">
         <v>9.0</v>
       </c>
       <c r="F118" s="31">
-        <v>11.0</v>
+        <v>18.0</v>
       </c>
       <c r="H118" s="6"/>
     </row>
     <row r="119">
       <c r="A119" s="6"/>
-      <c r="C119" s="28" t="s">
-        <v>27</v>
+      <c r="C119" s="32" t="s">
+        <v>32</v>
       </c>
       <c r="D119" s="26"/>
-      <c r="E119" s="29">
-        <v>9.0</v>
-      </c>
-      <c r="F119" s="29">
-        <v>16.0</v>
-      </c>
-      <c r="H119" s="6"/>
-    </row>
-    <row r="120">
-      <c r="A120" s="6"/>
-      <c r="C120" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D120" s="26"/>
-      <c r="E120" s="31">
-        <v>9.0</v>
-      </c>
-      <c r="F120" s="31">
-        <v>21.0</v>
-      </c>
-      <c r="H120" s="6"/>
-    </row>
-    <row r="121">
-      <c r="A121" s="6"/>
-      <c r="C121" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D121" s="26"/>
-      <c r="E121" s="29">
-        <v>10.0</v>
-      </c>
-      <c r="F121" s="29">
-        <v>12.0</v>
-      </c>
-      <c r="H121" s="6"/>
-    </row>
-    <row r="122">
-      <c r="A122" s="6"/>
-      <c r="C122" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D122" s="26"/>
-      <c r="E122" s="31">
-        <v>4.0</v>
-      </c>
-      <c r="F122" s="31">
-        <v>8.0</v>
-      </c>
-      <c r="H122" s="6"/>
-    </row>
-    <row r="123">
-      <c r="A123" s="6"/>
-      <c r="C123" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D123" s="26"/>
-      <c r="E123" s="29">
-        <v>9.0</v>
-      </c>
-      <c r="F123" s="29">
-        <v>13.0</v>
-      </c>
-      <c r="H123" s="6"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="6"/>
-      <c r="C124" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D124" s="26"/>
-      <c r="E124" s="31">
-        <v>9.0</v>
-      </c>
-      <c r="F124" s="31">
-        <v>18.0</v>
-      </c>
-      <c r="H124" s="6"/>
-    </row>
-    <row r="125">
-      <c r="A125" s="6"/>
-      <c r="C125" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D125" s="26"/>
-      <c r="E125" s="32">
-        <f t="shared" ref="E125:F125" si="1">sum(E117:E124)</f>
+      <c r="E119" s="33">
+        <f t="shared" ref="E119:F119" si="1">sum(E111:E118)</f>
         <v>63</v>
       </c>
-      <c r="F125" s="32">
+      <c r="F119" s="33">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="H125" s="6"/>
+      <c r="H119" s="6"/>
+    </row>
+    <row r="120">
+      <c r="B120" s="34"/>
+      <c r="C120" s="34"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="10"/>
+      <c r="B121" s="34"/>
+      <c r="C121" s="34"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="6"/>
-      <c r="B126" s="33"/>
-      <c r="C126" s="33"/>
+      <c r="B126" s="34"/>
+      <c r="C126" s="34"/>
       <c r="D126" s="6"/>
       <c r="E126" s="6"/>
       <c r="F126" s="6"/>
@@ -1484,8 +1528,8 @@
     </row>
     <row r="127">
       <c r="A127" s="6"/>
-      <c r="B127" s="33"/>
-      <c r="C127" s="33"/>
+      <c r="B127" s="34"/>
+      <c r="C127" s="34"/>
       <c r="D127" s="6"/>
       <c r="E127" s="6"/>
       <c r="F127" s="6"/>
@@ -1494,82 +1538,130 @@
     </row>
     <row r="128">
       <c r="A128" s="6"/>
-      <c r="B128" s="33"/>
-      <c r="C128" s="33"/>
-      <c r="D128" s="6"/>
-      <c r="E128" s="6"/>
-      <c r="F128" s="6"/>
-      <c r="G128" s="6"/>
+      <c r="B128" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C128" s="26"/>
+      <c r="D128" s="35"/>
+      <c r="E128" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F128" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G128" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="H128" s="6"/>
     </row>
     <row r="129">
       <c r="A129" s="6"/>
-      <c r="B129" s="33"/>
-      <c r="C129" s="33"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="6"/>
-      <c r="F129" s="6"/>
-      <c r="G129" s="6"/>
+      <c r="B129" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C129" s="26"/>
+      <c r="D129" s="35"/>
+      <c r="E129" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F129" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G129" s="29"/>
       <c r="H129" s="6"/>
     </row>
     <row r="130">
       <c r="A130" s="6"/>
-      <c r="B130" s="33"/>
-      <c r="C130" s="33"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="6"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="6"/>
+      <c r="B130" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C130" s="26"/>
+      <c r="D130" s="35"/>
+      <c r="E130" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F130" s="38">
+        <f>E119</f>
+        <v>63</v>
+      </c>
+      <c r="G130" s="31"/>
       <c r="H130" s="6"/>
     </row>
     <row r="131">
       <c r="A131" s="6"/>
-      <c r="B131" s="33"/>
-      <c r="C131" s="33"/>
-      <c r="D131" s="6"/>
-      <c r="E131" s="6"/>
-      <c r="F131" s="6"/>
-      <c r="G131" s="6"/>
+      <c r="B131" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C131" s="26"/>
+      <c r="D131" s="35"/>
+      <c r="E131" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F131" s="29">
+        <v>16.0</v>
+      </c>
+      <c r="G131" s="39"/>
       <c r="H131" s="6"/>
     </row>
     <row r="132">
       <c r="A132" s="6"/>
-      <c r="B132" s="33"/>
-      <c r="C132" s="33"/>
-      <c r="D132" s="6"/>
-      <c r="E132" s="6"/>
-      <c r="F132" s="6"/>
-      <c r="G132" s="6"/>
+      <c r="B132" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C132" s="26"/>
+      <c r="D132" s="35"/>
+      <c r="E132" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F132" s="38"/>
+      <c r="G132" s="38"/>
       <c r="H132" s="6"/>
     </row>
     <row r="133">
       <c r="A133" s="6"/>
-      <c r="B133" s="33"/>
-      <c r="C133" s="33"/>
-      <c r="D133" s="6"/>
-      <c r="E133" s="6"/>
-      <c r="F133" s="6"/>
-      <c r="G133" s="6"/>
+      <c r="B133" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C133" s="26"/>
+      <c r="D133" s="35"/>
+      <c r="E133" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F133" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G133" s="39"/>
       <c r="H133" s="6"/>
     </row>
     <row r="134">
       <c r="A134" s="6"/>
-      <c r="B134" s="33"/>
-      <c r="C134" s="33"/>
-      <c r="D134" s="6"/>
-      <c r="E134" s="6"/>
-      <c r="F134" s="6"/>
-      <c r="G134" s="6"/>
+      <c r="B134" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C134" s="26"/>
+      <c r="D134" s="35"/>
+      <c r="E134" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F134" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G134" s="38"/>
       <c r="H134" s="6"/>
     </row>
     <row r="135">
       <c r="A135" s="6"/>
-      <c r="B135" s="6"/>
-      <c r="C135" s="6"/>
-      <c r="D135" s="6"/>
-      <c r="E135" s="6"/>
-      <c r="F135" s="6"/>
-      <c r="G135" s="6"/>
+      <c r="B135" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C135" s="26"/>
+      <c r="D135" s="26"/>
+      <c r="E135" s="26"/>
+      <c r="F135" s="35"/>
+      <c r="G135" s="42">
+        <f>sum(G129:G134)</f>
+        <v>0</v>
+      </c>
       <c r="H135" s="6"/>
     </row>
     <row r="136">
@@ -1982,18 +2074,8 @@
       <c r="G176" s="6"/>
       <c r="H176" s="6"/>
     </row>
-    <row r="177">
-      <c r="A177" s="6"/>
-      <c r="B177" s="6"/>
-      <c r="C177" s="6"/>
-      <c r="D177" s="6"/>
-      <c r="E177" s="6"/>
-      <c r="F177" s="6"/>
-      <c r="G177" s="6"/>
-      <c r="H177" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="33">
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="A15:H18"/>
     <mergeCell ref="A24:C24"/>
@@ -2007,17 +2089,26 @@
     <mergeCell ref="A53:H56"/>
     <mergeCell ref="B73:H73"/>
     <mergeCell ref="B74:H75"/>
-    <mergeCell ref="A108:H111"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="A104:H107"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
     <mergeCell ref="C116:D116"/>
+    <mergeCell ref="B132:D132"/>
+    <mergeCell ref="B133:D133"/>
+    <mergeCell ref="B134:D134"/>
+    <mergeCell ref="B135:F135"/>
     <mergeCell ref="C117:D117"/>
     <mergeCell ref="C118:D118"/>
     <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="B131:D131"/>
+    <mergeCell ref="B129:D129"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="A122:H125"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
zmiana formatowania kosztorysu, zabiegi estetyczne
</commit_message>
<xml_diff>
--- a/kosztorys-wstepny.xlsx
+++ b/kosztorys-wstepny.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Wrocław, 15.01.2025r.</t>
   </si>
@@ -57,8 +57,10 @@
     <t>Podpis sporządzającego:</t>
   </si>
   <si>
-    <t>Montaż i instalacja lokalnej sieci komputerowej
- w budynku przy ulicy Zielonej w Warszawie</t>
+    <t>1. Ogólna charakterystyka prac objętych kosztorysem</t>
+  </si>
+  <si>
+    <t>Montaż i instalacja lokalnej sieci komputerowej w budynku przy ulicy Zielonej.</t>
   </si>
   <si>
     <t>1.1 Podstawa sporządzenia kosztorysu:</t>
@@ -85,8 +87,7 @@
     <t>- Montaż szafy dystrybucyjnej typu rack w rejestracji, wiszącej, w rozmiarze 12U.</t>
   </si>
   <si>
-    <t>Długości przewodów, które zostaną użyte
- do stworzenia lokalnej sieci komputerowej</t>
+    <t>2. Długości przewodów, które zostaną użyte do stworzenia sieci LAN</t>
   </si>
   <si>
     <t>Połączenie z ... do ...</t>
@@ -122,10 +123,10 @@
     <t>Rejestracja - gabinet nr 7</t>
   </si>
   <si>
-    <t>Razem</t>
-  </si>
-  <si>
-    <t>Przedmiar prac</t>
+    <t>Razem:</t>
+  </si>
+  <si>
+    <t>3. Przedmiar prac</t>
   </si>
   <si>
     <t>Nazwa</t>
@@ -166,16 +167,13 @@
   </si>
   <si>
     <t>Porządkowanie instalacji</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Razem:  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -226,31 +224,19 @@
     </font>
     <font>
       <b/>
+      <sz val="16.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18.0"/>
       <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
     <font>
-      <b/>
-      <sz val="21.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12.0"/>
-      <color rgb="FFC9211E"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <color rgb="FFC9211E"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18.0"/>
       <color rgb="FFC9211E"/>
       <name val="Liberation Sans"/>
     </font>
@@ -338,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -374,20 +360,14 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -397,26 +377,11 @@
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -431,35 +396,41 @@
     <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -673,7 +644,7 @@
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
@@ -939,562 +910,537 @@
       <c r="E43" s="11"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="10">
-        <v>1.0</v>
-      </c>
+      <c r="H43" s="10"/>
     </row>
     <row r="44">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+      <c r="A44" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="6"/>
+      <c r="A48" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="11"/>
+      <c r="E48" s="13"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="10"/>
     </row>
     <row r="49">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="10"/>
+      <c r="E49" s="14"/>
     </row>
     <row r="50">
-      <c r="A50" s="6"/>
+      <c r="A50" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
-      <c r="E50" s="11"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="10"/>
     </row>
     <row r="51">
       <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
-      <c r="E51" s="11"/>
+      <c r="E51" s="15"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="10"/>
     </row>
     <row r="52">
-      <c r="E52" s="12"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
     </row>
     <row r="53">
-      <c r="A53" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="A53" s="6"/>
+      <c r="B53" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="6"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
     </row>
     <row r="57">
-      <c r="E57" s="14"/>
+      <c r="A57" s="6"/>
+      <c r="B57" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="58">
-      <c r="E58" s="14"/>
+      <c r="A58" s="6"/>
+      <c r="B58" s="16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="59">
-      <c r="E59" s="15"/>
+      <c r="A59" s="6"/>
     </row>
     <row r="60">
+      <c r="A60" s="6"/>
+      <c r="B60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
       <c r="E60" s="15"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
     </row>
     <row r="61">
+      <c r="A61" s="6"/>
+      <c r="B61" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
       <c r="E61" s="15"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
     </row>
     <row r="62">
-      <c r="E62" s="15"/>
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
     </row>
     <row r="63">
-      <c r="E63" s="15"/>
-    </row>
-    <row r="64">
-      <c r="E64" s="15"/>
-    </row>
-    <row r="65">
-      <c r="E65" s="14"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="6"/>
-      <c r="G66" s="6"/>
+      <c r="A63" s="12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="6"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
+      <c r="C67" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="19"/>
+      <c r="E67" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H67" s="6"/>
     </row>
     <row r="68">
       <c r="A68" s="6"/>
-      <c r="B68" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
+      <c r="C68" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="19"/>
+      <c r="E68" s="22">
+        <v>4.0</v>
+      </c>
+      <c r="F68" s="22">
+        <v>6.0</v>
+      </c>
+      <c r="H68" s="6"/>
     </row>
     <row r="69">
       <c r="A69" s="6"/>
-      <c r="B69" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
+      <c r="C69" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" s="19"/>
+      <c r="E69" s="24">
+        <v>9.0</v>
+      </c>
+      <c r="F69" s="24">
+        <v>11.0</v>
+      </c>
+      <c r="H69" s="6"/>
     </row>
     <row r="70">
       <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
+      <c r="C70" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="19"/>
+      <c r="E70" s="22">
+        <v>9.0</v>
+      </c>
+      <c r="F70" s="22">
+        <v>16.0</v>
+      </c>
+      <c r="H70" s="6"/>
     </row>
     <row r="71">
-      <c r="A71" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
+      <c r="A71" s="6"/>
+      <c r="C71" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" s="19"/>
+      <c r="E71" s="24">
+        <v>9.0</v>
+      </c>
+      <c r="F71" s="24">
+        <v>21.0</v>
+      </c>
+      <c r="H71" s="6"/>
     </row>
     <row r="72">
       <c r="A72" s="6"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="10"/>
-      <c r="H72" s="10"/>
+      <c r="C72" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="19"/>
+      <c r="E72" s="22">
+        <v>10.0</v>
+      </c>
+      <c r="F72" s="22">
+        <v>12.0</v>
+      </c>
+      <c r="H72" s="6"/>
     </row>
     <row r="73">
       <c r="A73" s="6"/>
-      <c r="B73" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="C73" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="19"/>
+      <c r="E73" s="24">
+        <v>4.0</v>
+      </c>
+      <c r="F73" s="24">
+        <v>8.0</v>
+      </c>
+      <c r="H73" s="6"/>
     </row>
     <row r="74">
       <c r="A74" s="6"/>
-      <c r="B74" s="18" t="s">
-        <v>17</v>
-      </c>
+      <c r="C74" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="19"/>
+      <c r="E74" s="22">
+        <v>9.0</v>
+      </c>
+      <c r="F74" s="22">
+        <v>13.0</v>
+      </c>
+      <c r="H74" s="6"/>
     </row>
     <row r="75">
       <c r="A75" s="6"/>
+      <c r="C75" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" s="19"/>
+      <c r="E75" s="24">
+        <v>9.0</v>
+      </c>
+      <c r="F75" s="24">
+        <v>18.0</v>
+      </c>
+      <c r="H75" s="6"/>
     </row>
     <row r="76">
       <c r="A76" s="6"/>
-      <c r="B76" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
+      <c r="C76" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="19"/>
+      <c r="E76" s="26">
+        <f t="shared" ref="E76:F76" si="1">sum(E68:E75)</f>
+        <v>63</v>
+      </c>
+      <c r="F76" s="26">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="H76" s="6"/>
     </row>
     <row r="77">
-      <c r="A77" s="6"/>
-      <c r="B77" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="27"/>
     </row>
     <row r="78">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="6"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="6"/>
-      <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
+      <c r="A78" s="27" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="82">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
+      <c r="B82" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="19"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G82" s="20" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" s="6"/>
-      <c r="B83" s="6"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C83" s="19"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F83" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G83" s="22"/>
     </row>
     <row r="84">
       <c r="A84" s="6"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
+      <c r="B84" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84" s="19"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F84" s="31">
+        <f>E76</f>
+        <v>63</v>
+      </c>
+      <c r="G84" s="24"/>
     </row>
     <row r="85">
       <c r="A85" s="6"/>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="6"/>
-      <c r="G85" s="6"/>
+      <c r="B85" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C85" s="19"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F85" s="22">
+        <v>16.0</v>
+      </c>
+      <c r="G85" s="32"/>
     </row>
     <row r="86">
       <c r="A86" s="6"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="6"/>
-      <c r="G86" s="6"/>
+      <c r="B86" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C86" s="19"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" s="31"/>
+      <c r="G86" s="31"/>
     </row>
     <row r="87">
-      <c r="A87" s="6"/>
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
+      <c r="B87" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C87" s="19"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F87" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G87" s="32"/>
     </row>
     <row r="88">
-      <c r="A88" s="6"/>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="6"/>
-      <c r="G88" s="6"/>
+      <c r="A88" s="33"/>
+      <c r="B88" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C88" s="19"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="G88" s="31"/>
     </row>
     <row r="89">
-      <c r="A89" s="6"/>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="6"/>
-      <c r="G89" s="6"/>
+      <c r="A89" s="33"/>
+      <c r="B89" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="36">
+        <f>sum(G83:G88)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
-      <c r="E90" s="23"/>
-    </row>
-    <row r="98">
-      <c r="H98" s="24">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="10"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="6"/>
-      <c r="G99" s="6"/>
-      <c r="H99" s="6"/>
-    </row>
-    <row r="100">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="6"/>
-      <c r="G100" s="6"/>
-      <c r="H100" s="6"/>
-    </row>
-    <row r="101">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="6"/>
-      <c r="H101" s="10"/>
-    </row>
-    <row r="102">
-      <c r="A102" s="6"/>
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="6"/>
-      <c r="G102" s="6"/>
-      <c r="H102" s="10"/>
-    </row>
-    <row r="103">
-      <c r="E103" s="12"/>
+      <c r="A90" s="33"/>
+      <c r="B90" s="33"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="33"/>
+      <c r="G90" s="33"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="33"/>
+      <c r="B91" s="33"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="33"/>
+      <c r="E91" s="33"/>
+      <c r="F91" s="33"/>
+      <c r="G91" s="33"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="10"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="6"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
     </row>
     <row r="104">
-      <c r="A104" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="10"/>
-      <c r="B108" s="6"/>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="6"/>
-      <c r="F108" s="6"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="6"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="6"/>
-      <c r="B109" s="6"/>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
-      <c r="F109" s="6"/>
-      <c r="G109" s="6"/>
-      <c r="H109" s="6"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="10"/>
+      <c r="B105" s="37"/>
+      <c r="C105" s="37"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
     </row>
     <row r="110">
-      <c r="C110" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D110" s="26"/>
-      <c r="E110" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="F110" s="27" t="s">
-        <v>23</v>
-      </c>
+      <c r="A110" s="6"/>
+      <c r="B110" s="37"/>
+      <c r="C110" s="37"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
       <c r="H110" s="6"/>
     </row>
     <row r="111">
       <c r="A111" s="6"/>
-      <c r="C111" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D111" s="26"/>
-      <c r="E111" s="29">
-        <v>4.0</v>
-      </c>
-      <c r="F111" s="29">
-        <v>6.0</v>
-      </c>
+      <c r="B111" s="37"/>
+      <c r="C111" s="37"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
       <c r="H111" s="6"/>
     </row>
     <row r="112">
       <c r="A112" s="6"/>
-      <c r="C112" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D112" s="26"/>
-      <c r="E112" s="31">
-        <v>9.0</v>
-      </c>
-      <c r="F112" s="31">
-        <v>11.0</v>
-      </c>
       <c r="H112" s="6"/>
     </row>
     <row r="113">
       <c r="A113" s="6"/>
-      <c r="C113" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D113" s="26"/>
-      <c r="E113" s="29">
-        <v>9.0</v>
-      </c>
-      <c r="F113" s="29">
-        <v>16.0</v>
-      </c>
       <c r="H113" s="6"/>
     </row>
     <row r="114">
       <c r="A114" s="6"/>
-      <c r="C114" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D114" s="26"/>
-      <c r="E114" s="31">
-        <v>9.0</v>
-      </c>
-      <c r="F114" s="31">
-        <v>21.0</v>
-      </c>
       <c r="H114" s="6"/>
     </row>
     <row r="115">
       <c r="A115" s="6"/>
-      <c r="C115" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D115" s="26"/>
-      <c r="E115" s="29">
-        <v>10.0</v>
-      </c>
-      <c r="F115" s="29">
-        <v>12.0</v>
-      </c>
       <c r="H115" s="6"/>
     </row>
     <row r="116">
       <c r="A116" s="6"/>
-      <c r="C116" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D116" s="26"/>
-      <c r="E116" s="31">
-        <v>4.0</v>
-      </c>
-      <c r="F116" s="31">
-        <v>8.0</v>
-      </c>
       <c r="H116" s="6"/>
     </row>
     <row r="117">
       <c r="A117" s="6"/>
-      <c r="C117" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D117" s="26"/>
-      <c r="E117" s="29">
-        <v>9.0</v>
-      </c>
-      <c r="F117" s="29">
-        <v>13.0</v>
-      </c>
       <c r="H117" s="6"/>
     </row>
     <row r="118">
       <c r="A118" s="6"/>
-      <c r="C118" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="D118" s="26"/>
-      <c r="E118" s="31">
-        <v>9.0</v>
-      </c>
-      <c r="F118" s="31">
-        <v>18.0</v>
-      </c>
       <c r="H118" s="6"/>
     </row>
     <row r="119">
       <c r="A119" s="6"/>
-      <c r="C119" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D119" s="26"/>
-      <c r="E119" s="33">
-        <f t="shared" ref="E119:F119" si="1">sum(E111:E118)</f>
-        <v>63</v>
-      </c>
-      <c r="F119" s="33">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
       <c r="H119" s="6"/>
     </row>
     <row r="120">
-      <c r="B120" s="34"/>
-      <c r="C120" s="34"/>
+      <c r="A120" s="6"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
       <c r="F120" s="6"/>
@@ -1502,9 +1448,9 @@
       <c r="H120" s="6"/>
     </row>
     <row r="121">
-      <c r="A121" s="10"/>
-      <c r="B121" s="34"/>
-      <c r="C121" s="34"/>
+      <c r="A121" s="6"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
       <c r="F121" s="6"/>
@@ -1512,14 +1458,49 @@
       <c r="H121" s="6"/>
     </row>
     <row r="122">
-      <c r="A122" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="A122" s="6"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="6"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="6"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="6"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
     </row>
     <row r="126">
       <c r="A126" s="6"/>
-      <c r="B126" s="34"/>
-      <c r="C126" s="34"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
       <c r="D126" s="6"/>
       <c r="E126" s="6"/>
       <c r="F126" s="6"/>
@@ -1528,8 +1509,8 @@
     </row>
     <row r="127">
       <c r="A127" s="6"/>
-      <c r="B127" s="34"/>
-      <c r="C127" s="34"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
       <c r="D127" s="6"/>
       <c r="E127" s="6"/>
       <c r="F127" s="6"/>
@@ -1538,130 +1519,82 @@
     </row>
     <row r="128">
       <c r="A128" s="6"/>
-      <c r="B128" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C128" s="26"/>
-      <c r="D128" s="35"/>
-      <c r="E128" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F128" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="G128" s="27" t="s">
-        <v>37</v>
-      </c>
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
       <c r="H128" s="6"/>
     </row>
     <row r="129">
       <c r="A129" s="6"/>
-      <c r="B129" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C129" s="26"/>
-      <c r="D129" s="35"/>
-      <c r="E129" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F129" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="G129" s="29"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="6"/>
+      <c r="G129" s="6"/>
       <c r="H129" s="6"/>
     </row>
     <row r="130">
       <c r="A130" s="6"/>
-      <c r="B130" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C130" s="26"/>
-      <c r="D130" s="35"/>
-      <c r="E130" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F130" s="38">
-        <f>E119</f>
-        <v>63</v>
-      </c>
-      <c r="G130" s="31"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
       <c r="H130" s="6"/>
     </row>
     <row r="131">
       <c r="A131" s="6"/>
-      <c r="B131" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C131" s="26"/>
-      <c r="D131" s="35"/>
-      <c r="E131" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F131" s="29">
-        <v>16.0</v>
-      </c>
-      <c r="G131" s="39"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
       <c r="H131" s="6"/>
     </row>
     <row r="132">
       <c r="A132" s="6"/>
-      <c r="B132" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C132" s="26"/>
-      <c r="D132" s="35"/>
-      <c r="E132" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="F132" s="38"/>
-      <c r="G132" s="38"/>
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
       <c r="H132" s="6"/>
     </row>
     <row r="133">
       <c r="A133" s="6"/>
-      <c r="B133" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C133" s="26"/>
-      <c r="D133" s="35"/>
-      <c r="E133" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F133" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="G133" s="39"/>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
       <c r="H133" s="6"/>
     </row>
     <row r="134">
       <c r="A134" s="6"/>
-      <c r="B134" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C134" s="26"/>
-      <c r="D134" s="35"/>
-      <c r="E134" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F134" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="G134" s="38"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
       <c r="H134" s="6"/>
     </row>
     <row r="135">
       <c r="A135" s="6"/>
-      <c r="B135" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C135" s="26"/>
-      <c r="D135" s="26"/>
-      <c r="E135" s="26"/>
-      <c r="F135" s="35"/>
-      <c r="G135" s="42">
-        <f>sum(G129:G134)</f>
-        <v>0</v>
-      </c>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
       <c r="H135" s="6"/>
     </row>
     <row r="136">
@@ -1914,168 +1847,28 @@
       <c r="G160" s="6"/>
       <c r="H160" s="6"/>
     </row>
-    <row r="161">
-      <c r="A161" s="6"/>
-      <c r="B161" s="6"/>
-      <c r="C161" s="6"/>
-      <c r="D161" s="6"/>
-      <c r="E161" s="6"/>
-      <c r="F161" s="6"/>
-      <c r="G161" s="6"/>
-      <c r="H161" s="6"/>
-    </row>
-    <row r="162">
-      <c r="A162" s="6"/>
-      <c r="B162" s="6"/>
-      <c r="C162" s="6"/>
-      <c r="D162" s="6"/>
-      <c r="E162" s="6"/>
-      <c r="F162" s="6"/>
-      <c r="G162" s="6"/>
-      <c r="H162" s="6"/>
-    </row>
-    <row r="163">
-      <c r="A163" s="6"/>
-      <c r="B163" s="6"/>
-      <c r="C163" s="6"/>
-      <c r="D163" s="6"/>
-      <c r="E163" s="6"/>
-      <c r="F163" s="6"/>
-      <c r="G163" s="6"/>
-      <c r="H163" s="6"/>
-    </row>
-    <row r="164">
-      <c r="A164" s="6"/>
-      <c r="B164" s="6"/>
-      <c r="C164" s="6"/>
-      <c r="D164" s="6"/>
-      <c r="E164" s="6"/>
-      <c r="F164" s="6"/>
-      <c r="G164" s="6"/>
-      <c r="H164" s="6"/>
-    </row>
-    <row r="165">
-      <c r="A165" s="6"/>
-      <c r="B165" s="6"/>
-      <c r="C165" s="6"/>
-      <c r="D165" s="6"/>
-      <c r="E165" s="6"/>
-      <c r="F165" s="6"/>
-      <c r="G165" s="6"/>
-      <c r="H165" s="6"/>
-    </row>
-    <row r="166">
-      <c r="A166" s="6"/>
-      <c r="B166" s="6"/>
-      <c r="C166" s="6"/>
-      <c r="D166" s="6"/>
-      <c r="E166" s="6"/>
-      <c r="F166" s="6"/>
-      <c r="G166" s="6"/>
-      <c r="H166" s="6"/>
-    </row>
-    <row r="167">
-      <c r="A167" s="6"/>
-      <c r="B167" s="6"/>
-      <c r="C167" s="6"/>
-      <c r="D167" s="6"/>
-      <c r="E167" s="6"/>
-      <c r="F167" s="6"/>
-      <c r="G167" s="6"/>
-      <c r="H167" s="6"/>
-    </row>
-    <row r="168">
-      <c r="A168" s="6"/>
-      <c r="B168" s="6"/>
-      <c r="C168" s="6"/>
-      <c r="D168" s="6"/>
-      <c r="E168" s="6"/>
-      <c r="F168" s="6"/>
-      <c r="G168" s="6"/>
-      <c r="H168" s="6"/>
-    </row>
-    <row r="169">
-      <c r="A169" s="6"/>
-      <c r="B169" s="6"/>
-      <c r="C169" s="6"/>
-      <c r="D169" s="6"/>
-      <c r="E169" s="6"/>
-      <c r="F169" s="6"/>
-      <c r="G169" s="6"/>
-      <c r="H169" s="6"/>
-    </row>
-    <row r="170">
-      <c r="A170" s="6"/>
-      <c r="B170" s="6"/>
-      <c r="C170" s="6"/>
-      <c r="D170" s="6"/>
-      <c r="E170" s="6"/>
-      <c r="F170" s="6"/>
-      <c r="G170" s="6"/>
-      <c r="H170" s="6"/>
-    </row>
-    <row r="171">
-      <c r="A171" s="6"/>
-      <c r="B171" s="6"/>
-      <c r="C171" s="6"/>
-      <c r="D171" s="6"/>
-      <c r="E171" s="6"/>
-      <c r="F171" s="6"/>
-      <c r="G171" s="6"/>
-      <c r="H171" s="6"/>
-    </row>
-    <row r="172">
-      <c r="A172" s="6"/>
-      <c r="B172" s="6"/>
-      <c r="C172" s="6"/>
-      <c r="D172" s="6"/>
-      <c r="E172" s="6"/>
-      <c r="F172" s="6"/>
-      <c r="G172" s="6"/>
-      <c r="H172" s="6"/>
-    </row>
-    <row r="173">
-      <c r="A173" s="6"/>
-      <c r="B173" s="6"/>
-      <c r="C173" s="6"/>
-      <c r="D173" s="6"/>
-      <c r="E173" s="6"/>
-      <c r="F173" s="6"/>
-      <c r="G173" s="6"/>
-      <c r="H173" s="6"/>
-    </row>
-    <row r="174">
-      <c r="A174" s="6"/>
-      <c r="B174" s="6"/>
-      <c r="C174" s="6"/>
-      <c r="D174" s="6"/>
-      <c r="E174" s="6"/>
-      <c r="F174" s="6"/>
-      <c r="G174" s="6"/>
-      <c r="H174" s="6"/>
-    </row>
-    <row r="175">
-      <c r="A175" s="6"/>
-      <c r="B175" s="6"/>
-      <c r="C175" s="6"/>
-      <c r="D175" s="6"/>
-      <c r="E175" s="6"/>
-      <c r="F175" s="6"/>
-      <c r="G175" s="6"/>
-      <c r="H175" s="6"/>
-    </row>
-    <row r="176">
-      <c r="A176" s="6"/>
-      <c r="B176" s="6"/>
-      <c r="C176" s="6"/>
-      <c r="D176" s="6"/>
-      <c r="E176" s="6"/>
-      <c r="F176" s="6"/>
-      <c r="G176" s="6"/>
-      <c r="H176" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A63:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A78:H81"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A44:H47"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B58:H59"/>
+    <mergeCell ref="C76:D76"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="A15:H18"/>
     <mergeCell ref="A24:C24"/>
@@ -2083,32 +1876,12 @@
     <mergeCell ref="A25:C30"/>
     <mergeCell ref="F25:H30"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A53:H56"/>
-    <mergeCell ref="B73:H73"/>
-    <mergeCell ref="B74:H75"/>
-    <mergeCell ref="A104:H107"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="B132:D132"/>
-    <mergeCell ref="B133:D133"/>
-    <mergeCell ref="B134:D134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B131:D131"/>
-    <mergeCell ref="B129:D129"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="A122:H125"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
dodanie roboczogodzin do przedmiaru prac zgodnie z KNR
</commit_message>
<xml_diff>
--- a/kosztorys-wstepny.xlsx
+++ b/kosztorys-wstepny.xlsx
@@ -160,10 +160,10 @@
     <t>sztuka</t>
   </si>
   <si>
-    <t>Instalacja okablowania w patchpanelu oraz odpowiednie oznakowanie</t>
-  </si>
-  <si>
-    <t>Montaż patchpaneli, organizerów przewodów oraz listew zasilającyh w szafie typu rack</t>
+    <t>Instalacja okablowania w gniazdach i patchpanelu oraz odpowiednie oznakowanie</t>
+  </si>
+  <si>
+    <t>Montaż patchpanela, organizera przewodów oraz listwy zasilającej w szafie typu rack</t>
   </si>
   <si>
     <t>Porządkowanie instalacji</t>
@@ -1239,7 +1239,9 @@
       <c r="F83" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G83" s="22"/>
+      <c r="G83" s="22">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="6"/>
@@ -1255,7 +1257,10 @@
         <f>E76</f>
         <v>63</v>
       </c>
-      <c r="G84" s="24"/>
+      <c r="G84" s="24">
+        <f>0.2*F84</f>
+        <v>12.6</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="6"/>
@@ -1270,7 +1275,10 @@
       <c r="F85" s="22">
         <v>16.0</v>
       </c>
-      <c r="G85" s="32"/>
+      <c r="G85" s="32">
+        <f>0.3*F85</f>
+        <v>4.8</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="6"/>
@@ -1282,8 +1290,14 @@
       <c r="E86" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F86" s="31"/>
-      <c r="G86" s="31"/>
+      <c r="F86" s="24">
+        <f>F85*2+2</f>
+        <v>34</v>
+      </c>
+      <c r="G86" s="31">
+        <f>2*F86</f>
+        <v>68</v>
+      </c>
     </row>
     <row r="87">
       <c r="B87" s="29" t="s">
@@ -1297,7 +1311,9 @@
       <c r="F87" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G87" s="32"/>
+      <c r="G87" s="22">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="33"/>
@@ -1312,7 +1328,9 @@
       <c r="F88" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G88" s="31"/>
+      <c r="G88" s="24">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="33"/>
@@ -1325,7 +1343,7 @@
       <c r="F89" s="28"/>
       <c r="G89" s="36">
         <f>sum(G83:G88)</f>
-        <v>0</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="90">

</xml_diff>

<commit_message>
dodanie tabelki z bezpośrednim nakładem rzeczowym
</commit_message>
<xml_diff>
--- a/kosztorys-wstepny.xlsx
+++ b/kosztorys-wstepny.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Arkusz1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Kosztorys wstępny" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
   <si>
     <t>Wrocław, 15.01.2025r.</t>
   </si>
@@ -167,6 +167,52 @@
   </si>
   <si>
     <t>Porządkowanie instalacji</t>
+  </si>
+  <si>
+    <t>4. Bezpośrednie nakłady rzeczowe</t>
+  </si>
+  <si>
+    <t>Jednostka</t>
+  </si>
+  <si>
+    <t>Szafa typu rack</t>
+  </si>
+  <si>
+    <t>Szafa instalacyjna rack wisząca 19" 12U</t>
+  </si>
+  <si>
+    <t>Patchpanel 19"/1U kat. 6, ekranowany, 24 porty</t>
+  </si>
+  <si>
+    <t>Organizer poziomy przewodów 19"/1U - grzebieniowy
+z listwą zaślepiającą</t>
+  </si>
+  <si>
+    <t>Patchcordy 0,5 m kat. 6</t>
+  </si>
+  <si>
+    <t>Półka na dokumentację</t>
+  </si>
+  <si>
+    <t>Listwa zasilająca</t>
+  </si>
+  <si>
+    <t>Przewody do sieci komputerowej, gniazda, kanały</t>
+  </si>
+  <si>
+    <t>Przewód F/UDP kat. 6, drut</t>
+  </si>
+  <si>
+    <t>Gniazdo sieciowe podwójne natynkowe 2*RJ-45</t>
+  </si>
+  <si>
+    <t>Kanały kablowe PCV 2 m, 25x40</t>
+  </si>
+  <si>
+    <t>Elementy dodatkowe</t>
+  </si>
+  <si>
+    <t>Opaska zaciskowa</t>
   </si>
 </sst>
 </file>
@@ -237,16 +283,17 @@
     </font>
     <font>
       <sz val="12.0"/>
-      <color rgb="FFC9211E"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font/>
+    <font>
+      <b/>
+      <sz val="16.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -324,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -374,14 +421,11 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -396,16 +440,16 @@
     <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -424,10 +468,19 @@
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="2" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -1041,402 +1094,539 @@
       <c r="G61" s="6"/>
     </row>
     <row r="62">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="12" t="s">
+      <c r="A62" s="12" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="66">
+      <c r="C66" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="18"/>
+      <c r="E66" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H66" s="6"/>
+    </row>
     <row r="67">
-      <c r="C67" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" s="19"/>
-      <c r="E67" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F67" s="20" t="s">
+      <c r="A67" s="6"/>
+      <c r="C67" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67" s="18"/>
+      <c r="E67" s="21">
+        <v>4.0</v>
+      </c>
+      <c r="F67" s="21">
+        <f>4*6</f>
         <v>24</v>
       </c>
       <c r="H67" s="6"/>
     </row>
     <row r="68">
       <c r="A68" s="6"/>
-      <c r="C68" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D68" s="19"/>
-      <c r="E68" s="22">
-        <v>4.0</v>
-      </c>
-      <c r="F68" s="22">
-        <v>6.0</v>
+      <c r="C68" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="18"/>
+      <c r="E68" s="23">
+        <v>9.0</v>
+      </c>
+      <c r="F68" s="23">
+        <f>2*11</f>
+        <v>22</v>
       </c>
       <c r="H68" s="6"/>
     </row>
     <row r="69">
       <c r="A69" s="6"/>
-      <c r="C69" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="24">
+      <c r="C69" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="18"/>
+      <c r="E69" s="21">
         <v>9.0</v>
       </c>
-      <c r="F69" s="24">
-        <v>11.0</v>
+      <c r="F69" s="21">
+        <f>2*16</f>
+        <v>32</v>
       </c>
       <c r="H69" s="6"/>
     </row>
     <row r="70">
       <c r="A70" s="6"/>
-      <c r="C70" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D70" s="19"/>
-      <c r="E70" s="22">
+      <c r="C70" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" s="18"/>
+      <c r="E70" s="23">
         <v>9.0</v>
       </c>
-      <c r="F70" s="22">
-        <v>16.0</v>
+      <c r="F70" s="23">
+        <f>2*21</f>
+        <v>42</v>
       </c>
       <c r="H70" s="6"/>
     </row>
     <row r="71">
       <c r="A71" s="6"/>
-      <c r="C71" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="24">
-        <v>9.0</v>
-      </c>
-      <c r="F71" s="24">
-        <v>21.0</v>
+      <c r="C71" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" s="18"/>
+      <c r="E71" s="21">
+        <v>10.0</v>
+      </c>
+      <c r="F71" s="21">
+        <f>2*12</f>
+        <v>24</v>
       </c>
       <c r="H71" s="6"/>
     </row>
     <row r="72">
       <c r="A72" s="6"/>
-      <c r="C72" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D72" s="19"/>
-      <c r="E72" s="22">
-        <v>10.0</v>
-      </c>
-      <c r="F72" s="22">
-        <v>12.0</v>
+      <c r="C72" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="23">
+        <v>4.0</v>
+      </c>
+      <c r="F72" s="23">
+        <f>2*8</f>
+        <v>16</v>
       </c>
       <c r="H72" s="6"/>
     </row>
     <row r="73">
       <c r="A73" s="6"/>
-      <c r="C73" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D73" s="19"/>
-      <c r="E73" s="24">
-        <v>4.0</v>
-      </c>
-      <c r="F73" s="24">
-        <v>8.0</v>
+      <c r="C73" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" s="18"/>
+      <c r="E73" s="21">
+        <v>9.0</v>
+      </c>
+      <c r="F73" s="21">
+        <f>2*13</f>
+        <v>26</v>
       </c>
       <c r="H73" s="6"/>
     </row>
     <row r="74">
       <c r="A74" s="6"/>
-      <c r="C74" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D74" s="19"/>
-      <c r="E74" s="22">
+      <c r="C74" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" s="18"/>
+      <c r="E74" s="23">
         <v>9.0</v>
       </c>
-      <c r="F74" s="22">
-        <v>13.0</v>
+      <c r="F74" s="23">
+        <f>2*18</f>
+        <v>36</v>
       </c>
       <c r="H74" s="6"/>
     </row>
     <row r="75">
       <c r="A75" s="6"/>
-      <c r="C75" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D75" s="19"/>
-      <c r="E75" s="24">
-        <v>9.0</v>
-      </c>
-      <c r="F75" s="24">
-        <v>18.0</v>
+      <c r="C75" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" s="18"/>
+      <c r="E75" s="25">
+        <f t="shared" ref="E75:F75" si="1">sum(E67:E74)</f>
+        <v>63</v>
+      </c>
+      <c r="F75" s="25">
+        <f t="shared" si="1"/>
+        <v>222</v>
       </c>
       <c r="H75" s="6"/>
     </row>
     <row r="76">
-      <c r="A76" s="6"/>
-      <c r="C76" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D76" s="19"/>
-      <c r="E76" s="26">
-        <f t="shared" ref="E76:F76" si="1">sum(E68:E75)</f>
+      <c r="A76" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" s="18"/>
+      <c r="D80" s="27"/>
+      <c r="E80" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G80" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="10"/>
+      <c r="B81" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" s="18"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F81" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G81" s="21">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="6"/>
+      <c r="B82" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C82" s="18"/>
+      <c r="D82" s="27"/>
+      <c r="E82" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F82" s="30">
+        <f>E75</f>
         <v>63</v>
       </c>
-      <c r="F76" s="26">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="H76" s="6"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="27"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="B82" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C82" s="19"/>
-      <c r="D82" s="28"/>
-      <c r="E82" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F82" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G82" s="20" t="s">
-        <v>38</v>
+      <c r="G82" s="23">
+        <f>0.2*F82</f>
+        <v>12.6</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="10"/>
-      <c r="B83" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C83" s="19"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F83" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G83" s="22">
-        <v>3.0</v>
+      <c r="A83" s="6"/>
+      <c r="B83" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C83" s="18"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F83" s="21">
+        <v>16.0</v>
+      </c>
+      <c r="G83" s="31">
+        <f>0.3*F83</f>
+        <v>4.8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="6"/>
-      <c r="B84" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C84" s="19"/>
-      <c r="D84" s="28"/>
-      <c r="E84" s="24" t="s">
+      <c r="B84" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C84" s="18"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F84" s="23">
+        <f>F83*2+2</f>
+        <v>34</v>
+      </c>
+      <c r="G84" s="30">
+        <f>F84</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C85" s="18"/>
+      <c r="D85" s="27"/>
+      <c r="E85" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F85" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G85" s="21">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="32"/>
+      <c r="B86" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C86" s="18"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F86" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G86" s="23">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="32"/>
+      <c r="B87" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="35">
+        <f>sum(G81:G86)</f>
+        <v>57.4</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="36"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="36"/>
+      <c r="F88" s="36"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="36"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="36"/>
+      <c r="B89" s="36"/>
+      <c r="C89" s="36"/>
+      <c r="D89" s="36"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="36"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="36"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G95" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="27"/>
+    </row>
+    <row r="97">
+      <c r="B97" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G97" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G98" s="23">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G99" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G100" s="23">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G101" s="21">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G102" s="23">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="27"/>
+    </row>
+    <row r="104">
+      <c r="B104" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F84" s="31">
-        <f>E76</f>
+      <c r="G104" s="23">
+        <f>F75</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G105" s="21">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G106" s="23">
+        <f>E75</f>
         <v>63</v>
       </c>
-      <c r="G84" s="24">
-        <f>0.2*F84</f>
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="6"/>
-      <c r="B85" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C85" s="19"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="22" t="s">
+    </row>
+    <row r="107">
+      <c r="B107" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
+      <c r="F107" s="18"/>
+      <c r="G107" s="27"/>
+    </row>
+    <row r="108">
+      <c r="B108" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F85" s="22">
-        <v>16.0</v>
-      </c>
-      <c r="G85" s="32">
-        <f>0.3*F85</f>
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="6"/>
-      <c r="B86" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C86" s="19"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F86" s="24">
-        <f>F85*2+2</f>
-        <v>34</v>
-      </c>
-      <c r="G86" s="31">
-        <f>2*F86</f>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="B87" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C87" s="19"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F87" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G87" s="22">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="33"/>
-      <c r="B88" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C88" s="19"/>
-      <c r="D88" s="28"/>
-      <c r="E88" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F88" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="G88" s="24">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="33"/>
-      <c r="B89" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C89" s="19"/>
-      <c r="D89" s="19"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="28"/>
-      <c r="G89" s="36">
-        <f>sum(G83:G88)</f>
-        <v>91.4</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="33"/>
-      <c r="B90" s="33"/>
-      <c r="C90" s="33"/>
-      <c r="D90" s="33"/>
-      <c r="E90" s="33"/>
-      <c r="F90" s="33"/>
-      <c r="G90" s="33"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="33"/>
-      <c r="B91" s="33"/>
-      <c r="C91" s="33"/>
-      <c r="D91" s="33"/>
-      <c r="E91" s="33"/>
-      <c r="F91" s="33"/>
-      <c r="G91" s="33"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="10"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="6"/>
-      <c r="G93" s="6"/>
-      <c r="H93" s="6"/>
-    </row>
-    <row r="104">
-      <c r="B104" s="37"/>
-      <c r="C104" s="37"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="6"/>
-      <c r="H104" s="6"/>
-    </row>
-    <row r="105">
-      <c r="A105" s="10"/>
-      <c r="B105" s="37"/>
-      <c r="C105" s="37"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
-    </row>
-    <row r="110">
-      <c r="A110" s="6"/>
-      <c r="B110" s="37"/>
-      <c r="C110" s="37"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="6"/>
-      <c r="F110" s="6"/>
-      <c r="G110" s="6"/>
-      <c r="H110" s="6"/>
-    </row>
-    <row r="111">
-      <c r="A111" s="6"/>
-      <c r="B111" s="37"/>
-      <c r="C111" s="37"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
-      <c r="F111" s="6"/>
-      <c r="G111" s="6"/>
-      <c r="H111" s="6"/>
-    </row>
-    <row r="112">
-      <c r="A112" s="6"/>
-      <c r="H112" s="6"/>
-    </row>
-    <row r="113">
-      <c r="A113" s="6"/>
-      <c r="H113" s="6"/>
+      <c r="G108" s="23">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="10"/>
+      <c r="B109" s="39"/>
+      <c r="C109" s="39"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
     </row>
     <row r="114">
       <c r="A114" s="6"/>
+      <c r="B114" s="39"/>
+      <c r="C114" s="39"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
       <c r="H114" s="6"/>
     </row>
     <row r="115">
       <c r="A115" s="6"/>
+      <c r="B115" s="39"/>
+      <c r="C115" s="39"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
       <c r="H115" s="6"/>
     </row>
     <row r="116">
@@ -1457,42 +1647,18 @@
     </row>
     <row r="120">
       <c r="A120" s="6"/>
-      <c r="B120" s="6"/>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
-      <c r="F120" s="6"/>
-      <c r="G120" s="6"/>
       <c r="H120" s="6"/>
     </row>
     <row r="121">
       <c r="A121" s="6"/>
-      <c r="B121" s="6"/>
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="6"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="6"/>
       <c r="H121" s="6"/>
     </row>
     <row r="122">
       <c r="A122" s="6"/>
-      <c r="B122" s="6"/>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="6"/>
       <c r="H122" s="6"/>
     </row>
     <row r="123">
       <c r="A123" s="6"/>
-      <c r="B123" s="6"/>
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="6"/>
-      <c r="F123" s="6"/>
-      <c r="G123" s="6"/>
       <c r="H123" s="6"/>
     </row>
     <row r="124">
@@ -1865,28 +2031,65 @@
       <c r="G160" s="6"/>
       <c r="H160" s="6"/>
     </row>
+    <row r="161">
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="6"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="6"/>
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="6"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="A63:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A78:H81"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B89:F89"/>
+  <mergeCells count="48">
+    <mergeCell ref="B95:E95"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="A90:H94"/>
+    <mergeCell ref="B97:E97"/>
+    <mergeCell ref="B98:E98"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="B100:E100"/>
+    <mergeCell ref="B83:D83"/>
     <mergeCell ref="B84:D84"/>
     <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A44:H47"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="B58:H59"/>
-    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="B102:E102"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="B106:E106"/>
+    <mergeCell ref="B107:G107"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="A15:H18"/>
     <mergeCell ref="A24:C24"/>
@@ -1894,12 +2097,30 @@
     <mergeCell ref="A25:C30"/>
     <mergeCell ref="F25:H30"/>
     <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A44:H47"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B58:H59"/>
+    <mergeCell ref="A62:H65"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A76:H79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="C71:D71"/>
     <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="B108:E108"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="B105:E105"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
dodanie wyceny wartości nakładów rzeczowych oraz pozostałych składników
</commit_message>
<xml_diff>
--- a/kosztorys-wstepny.xlsx
+++ b/kosztorys-wstepny.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
   <si>
     <t>Wrocław, 15.01.2025r.</t>
   </si>
@@ -214,11 +214,33 @@
   <si>
     <t>Opaska zaciskowa</t>
   </si>
+  <si>
+    <t>5. Wycena wartości nakładów rzeczowych oraz pozostałych składników kalkulacyjnych ceny kosztorysowej</t>
+  </si>
+  <si>
+    <t>Cena jednostkowa</t>
+  </si>
+  <si>
+    <t>Wartość</t>
+  </si>
+  <si>
+    <t>Robocizna</t>
+  </si>
+  <si>
+    <t>Instalator-monter</t>
+  </si>
+  <si>
+    <t>roboczo-
+godzina</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$zł-415]"/>
+  </numFmts>
   <fonts count="13">
     <font>
       <sz val="10.0"/>
@@ -371,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="48">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -406,6 +428,7 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -481,9 +504,28 @@
     <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="10" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -845,7 +887,10 @@
       <c r="A32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="6"/>
+      <c r="C32" s="12">
+        <f>H131</f>
+        <v>5249.5</v>
+      </c>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="6"/>
@@ -966,7 +1011,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -977,12 +1022,12 @@
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="13"/>
+      <c r="E48" s="14"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
     <row r="49">
-      <c r="E49" s="14"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50">
       <c r="A50" s="10" t="s">
@@ -991,7 +1036,7 @@
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
-      <c r="E50" s="13"/>
+      <c r="E50" s="14"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
@@ -1000,7 +1045,7 @@
       <c r="B51" s="10"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
-      <c r="E51" s="15"/>
+      <c r="E51" s="16"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
@@ -1011,7 +1056,7 @@
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="15"/>
+      <c r="E52" s="16"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
     </row>
@@ -1022,7 +1067,7 @@
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
-      <c r="E53" s="13"/>
+      <c r="E53" s="14"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
     </row>
@@ -1031,7 +1076,7 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
-      <c r="E54" s="15"/>
+      <c r="E54" s="16"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
@@ -1042,7 +1087,7 @@
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
-      <c r="E55" s="13"/>
+      <c r="E55" s="14"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
@@ -1064,7 +1109,7 @@
     </row>
     <row r="58">
       <c r="A58" s="6"/>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1078,7 +1123,7 @@
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
-      <c r="E60" s="15"/>
+      <c r="E60" s="16"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
@@ -1089,38 +1134,38 @@
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="15"/>
+      <c r="E61" s="16"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
     <row r="62">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="66">
-      <c r="C66" s="17" t="s">
+      <c r="C66" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D66" s="18"/>
-      <c r="E66" s="19" t="s">
+      <c r="D66" s="19"/>
+      <c r="E66" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F66" s="19" t="s">
+      <c r="F66" s="20" t="s">
         <v>24</v>
       </c>
       <c r="H66" s="6"/>
     </row>
     <row r="67">
       <c r="A67" s="6"/>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D67" s="18"/>
-      <c r="E67" s="21">
+      <c r="D67" s="19"/>
+      <c r="E67" s="22">
         <v>4.0</v>
       </c>
-      <c r="F67" s="21">
+      <c r="F67" s="22">
         <f>4*6</f>
         <v>24</v>
       </c>
@@ -1128,14 +1173,14 @@
     </row>
     <row r="68">
       <c r="A68" s="6"/>
-      <c r="C68" s="22" t="s">
+      <c r="C68" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D68" s="18"/>
-      <c r="E68" s="23">
+      <c r="D68" s="19"/>
+      <c r="E68" s="24">
         <v>9.0</v>
       </c>
-      <c r="F68" s="23">
+      <c r="F68" s="24">
         <f>2*11</f>
         <v>22</v>
       </c>
@@ -1143,14 +1188,14 @@
     </row>
     <row r="69">
       <c r="A69" s="6"/>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D69" s="18"/>
-      <c r="E69" s="21">
+      <c r="D69" s="19"/>
+      <c r="E69" s="22">
         <v>9.0</v>
       </c>
-      <c r="F69" s="21">
+      <c r="F69" s="22">
         <f>2*16</f>
         <v>32</v>
       </c>
@@ -1158,14 +1203,14 @@
     </row>
     <row r="70">
       <c r="A70" s="6"/>
-      <c r="C70" s="22" t="s">
+      <c r="C70" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D70" s="18"/>
-      <c r="E70" s="23">
+      <c r="D70" s="19"/>
+      <c r="E70" s="24">
         <v>9.0</v>
       </c>
-      <c r="F70" s="23">
+      <c r="F70" s="24">
         <f>2*21</f>
         <v>42</v>
       </c>
@@ -1173,14 +1218,14 @@
     </row>
     <row r="71">
       <c r="A71" s="6"/>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D71" s="18"/>
-      <c r="E71" s="21">
+      <c r="D71" s="19"/>
+      <c r="E71" s="22">
         <v>10.0</v>
       </c>
-      <c r="F71" s="21">
+      <c r="F71" s="22">
         <f>2*12</f>
         <v>24</v>
       </c>
@@ -1188,14 +1233,14 @@
     </row>
     <row r="72">
       <c r="A72" s="6"/>
-      <c r="C72" s="22" t="s">
+      <c r="C72" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D72" s="18"/>
-      <c r="E72" s="23">
+      <c r="D72" s="19"/>
+      <c r="E72" s="24">
         <v>4.0</v>
       </c>
-      <c r="F72" s="23">
+      <c r="F72" s="24">
         <f>2*8</f>
         <v>16</v>
       </c>
@@ -1203,14 +1248,14 @@
     </row>
     <row r="73">
       <c r="A73" s="6"/>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D73" s="18"/>
-      <c r="E73" s="21">
+      <c r="D73" s="19"/>
+      <c r="E73" s="22">
         <v>9.0</v>
       </c>
-      <c r="F73" s="21">
+      <c r="F73" s="22">
         <f>2*13</f>
         <v>26</v>
       </c>
@@ -1218,14 +1263,14 @@
     </row>
     <row r="74">
       <c r="A74" s="6"/>
-      <c r="C74" s="22" t="s">
+      <c r="C74" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="23">
+      <c r="D74" s="19"/>
+      <c r="E74" s="24">
         <v>9.0</v>
       </c>
-      <c r="F74" s="23">
+      <c r="F74" s="24">
         <f>2*18</f>
         <v>36</v>
       </c>
@@ -1233,513 +1278,721 @@
     </row>
     <row r="75">
       <c r="A75" s="6"/>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="25">
+      <c r="D75" s="19"/>
+      <c r="E75" s="26">
         <f t="shared" ref="E75:F75" si="1">sum(E67:E74)</f>
         <v>63</v>
       </c>
-      <c r="F75" s="25">
+      <c r="F75" s="26">
         <f t="shared" si="1"/>
         <v>222</v>
       </c>
       <c r="H75" s="6"/>
     </row>
     <row r="76">
-      <c r="A76" s="26" t="s">
+      <c r="A76" s="27" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="80">
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C80" s="18"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="19" t="s">
+      <c r="C80" s="19"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F80" s="19" t="s">
+      <c r="F80" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G80" s="19" t="s">
+      <c r="G80" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="10"/>
-      <c r="B81" s="28" t="s">
+      <c r="B81" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C81" s="18"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="21" t="s">
+      <c r="C81" s="19"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F81" s="21" t="s">
+      <c r="F81" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G81" s="21">
+      <c r="G81" s="22">
         <v>3.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="6"/>
-      <c r="B82" s="29" t="s">
+      <c r="B82" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C82" s="18"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="23" t="s">
+      <c r="C82" s="19"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F82" s="30">
+      <c r="F82" s="31">
         <f>E75</f>
         <v>63</v>
       </c>
-      <c r="G82" s="23">
+      <c r="G82" s="24">
         <f>0.2*F82</f>
         <v>12.6</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="6"/>
-      <c r="B83" s="28" t="s">
+      <c r="B83" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C83" s="18"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="21" t="s">
+      <c r="C83" s="19"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F83" s="21">
+      <c r="F83" s="22">
         <v>16.0</v>
       </c>
-      <c r="G83" s="31">
+      <c r="G83" s="32">
         <f>0.3*F83</f>
         <v>4.8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="6"/>
-      <c r="B84" s="29" t="s">
+      <c r="B84" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C84" s="18"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="23" t="s">
+      <c r="C84" s="19"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F84" s="23">
+      <c r="F84" s="24">
         <f>F83*2+2</f>
         <v>34</v>
       </c>
-      <c r="G84" s="30">
+      <c r="G84" s="31">
         <f>F84</f>
         <v>34</v>
       </c>
     </row>
     <row r="85">
-      <c r="B85" s="28" t="s">
+      <c r="B85" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C85" s="18"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="21" t="s">
+      <c r="C85" s="19"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F85" s="21" t="s">
+      <c r="F85" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G85" s="21">
+      <c r="G85" s="22">
         <v>2.0</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="32"/>
-      <c r="B86" s="33" t="s">
+      <c r="A86" s="33"/>
+      <c r="B86" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C86" s="18"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="23" t="s">
+      <c r="C86" s="19"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F86" s="23" t="s">
+      <c r="F86" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G86" s="23">
+      <c r="G86" s="24">
         <v>1.0</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="32"/>
-      <c r="B87" s="34" t="s">
+      <c r="A87" s="33"/>
+      <c r="B87" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="35">
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="36">
         <f>sum(G81:G86)</f>
         <v>57.4</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="36"/>
-      <c r="B88" s="36"/>
-      <c r="C88" s="36"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="36"/>
-      <c r="F88" s="36"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="36"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
     </row>
     <row r="89">
-      <c r="A89" s="36"/>
-      <c r="B89" s="36"/>
-      <c r="C89" s="36"/>
-      <c r="D89" s="36"/>
-      <c r="E89" s="36"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="36"/>
-      <c r="H89" s="36"/>
+      <c r="A89" s="37"/>
+      <c r="B89" s="37"/>
+      <c r="C89" s="37"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="37"/>
+      <c r="G89" s="37"/>
+      <c r="H89" s="37"/>
     </row>
     <row r="90">
-      <c r="A90" s="36" t="s">
+      <c r="A90" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="95">
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="19" t="s">
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G95" s="19" t="s">
+      <c r="G95" s="20" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="96">
-      <c r="B96" s="37" t="s">
+      <c r="B96" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C96" s="18"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
-      <c r="F96" s="18"/>
-      <c r="G96" s="27"/>
+      <c r="C96" s="19"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="19"/>
+      <c r="G96" s="28"/>
     </row>
     <row r="97">
-      <c r="B97" s="20" t="s">
+      <c r="B97" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="21" t="s">
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G97" s="21">
+      <c r="G97" s="22">
         <v>1.0</v>
       </c>
     </row>
     <row r="98">
-      <c r="B98" s="22" t="s">
+      <c r="B98" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C98" s="18"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="23" t="s">
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G98" s="23">
+      <c r="G98" s="24">
         <v>1.0</v>
       </c>
     </row>
     <row r="99">
-      <c r="B99" s="20" t="s">
+      <c r="B99" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C99" s="18"/>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18"/>
-      <c r="F99" s="21" t="s">
+      <c r="C99" s="19"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G99" s="21">
+      <c r="G99" s="22">
         <v>1.0</v>
       </c>
     </row>
     <row r="100">
-      <c r="B100" s="22" t="s">
+      <c r="B100" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="23" t="s">
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G100" s="23">
+      <c r="G100" s="24">
         <v>18.0</v>
       </c>
     </row>
     <row r="101">
-      <c r="B101" s="20" t="s">
+      <c r="B101" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="21" t="s">
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G101" s="21">
+      <c r="G101" s="22">
         <v>1.0</v>
       </c>
     </row>
     <row r="102">
-      <c r="B102" s="22" t="s">
+      <c r="B102" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="23" t="s">
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G102" s="23">
+      <c r="G102" s="24">
         <v>1.0</v>
       </c>
     </row>
     <row r="103">
-      <c r="B103" s="38" t="s">
+      <c r="B103" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="18"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="27"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="28"/>
     </row>
     <row r="104">
-      <c r="B104" s="22" t="s">
+      <c r="B104" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C104" s="18"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="23" t="s">
+      <c r="C104" s="19"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G104" s="23">
+      <c r="G104" s="24">
         <f>F75</f>
         <v>222</v>
       </c>
     </row>
     <row r="105">
-      <c r="B105" s="20" t="s">
+      <c r="B105" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C105" s="18"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="21" t="s">
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G105" s="21">
+      <c r="G105" s="22">
         <v>9.0</v>
       </c>
     </row>
     <row r="106">
-      <c r="B106" s="22" t="s">
+      <c r="B106" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C106" s="18"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="23" t="s">
+      <c r="C106" s="19"/>
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G106" s="23">
+      <c r="G106" s="24">
         <f>E75</f>
         <v>63</v>
       </c>
     </row>
     <row r="107">
-      <c r="B107" s="38" t="s">
+      <c r="B107" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C107" s="18"/>
-      <c r="D107" s="18"/>
-      <c r="E107" s="18"/>
-      <c r="F107" s="18"/>
-      <c r="G107" s="27"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="28"/>
     </row>
     <row r="108">
-      <c r="B108" s="22" t="s">
+      <c r="B108" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C108" s="18"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="23" t="s">
+      <c r="C108" s="19"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G108" s="23">
+      <c r="G108" s="24">
         <v>100.0</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="10"/>
-      <c r="B109" s="39"/>
-      <c r="C109" s="39"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
-      <c r="F109" s="6"/>
-      <c r="G109" s="6"/>
-      <c r="H109" s="6"/>
+      <c r="A109" s="40"/>
+      <c r="B109" s="40"/>
+      <c r="C109" s="40"/>
+      <c r="D109" s="40"/>
+      <c r="E109" s="40"/>
+      <c r="F109" s="40"/>
+      <c r="G109" s="40"/>
+      <c r="H109" s="40"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="40" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="114">
-      <c r="A114" s="6"/>
-      <c r="B114" s="39"/>
-      <c r="C114" s="39"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="6"/>
-      <c r="F114" s="6"/>
-      <c r="G114" s="6"/>
-      <c r="H114" s="6"/>
+      <c r="A114" s="40"/>
+      <c r="B114" s="40"/>
+      <c r="C114" s="40"/>
+      <c r="D114" s="40"/>
+      <c r="E114" s="40"/>
+      <c r="F114" s="40"/>
+      <c r="G114" s="40"/>
+      <c r="H114" s="40"/>
     </row>
     <row r="115">
-      <c r="A115" s="6"/>
-      <c r="B115" s="39"/>
-      <c r="C115" s="39"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="6"/>
-      <c r="F115" s="6"/>
-      <c r="G115" s="6"/>
-      <c r="H115" s="6"/>
+      <c r="A115" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B115" s="19"/>
+      <c r="C115" s="19"/>
+      <c r="D115" s="28"/>
+      <c r="E115" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F115" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G115" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H115" s="20" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="116">
-      <c r="A116" s="6"/>
-      <c r="H116" s="6"/>
+      <c r="A116" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B116" s="19"/>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="19"/>
+      <c r="H116" s="28"/>
     </row>
     <row r="117">
-      <c r="A117" s="6"/>
-      <c r="H117" s="6"/>
+      <c r="A117" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B117" s="19"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F117" s="41">
+        <v>50.0</v>
+      </c>
+      <c r="G117" s="22">
+        <f>G87</f>
+        <v>57.4</v>
+      </c>
+      <c r="H117" s="41">
+        <f>F117*G117</f>
+        <v>2870</v>
+      </c>
     </row>
     <row r="118">
-      <c r="A118" s="6"/>
-      <c r="H118" s="6"/>
+      <c r="A118" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B118" s="19"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="28"/>
     </row>
     <row r="119">
-      <c r="A119" s="6"/>
-      <c r="H119" s="6"/>
+      <c r="A119" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F119" s="41">
+        <v>525.0</v>
+      </c>
+      <c r="G119" s="42">
+        <f t="shared" ref="G119:G124" si="2">G97</f>
+        <v>1</v>
+      </c>
+      <c r="H119" s="43">
+        <f t="shared" ref="H119:H124" si="3">G119*F119</f>
+        <v>525</v>
+      </c>
     </row>
     <row r="120">
-      <c r="A120" s="6"/>
-      <c r="H120" s="6"/>
+      <c r="A120" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B120" s="19"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="28"/>
+      <c r="E120" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F120" s="44">
+        <v>150.0</v>
+      </c>
+      <c r="G120" s="45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H120" s="46">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="121">
-      <c r="A121" s="6"/>
-      <c r="H121" s="6"/>
+      <c r="A121" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B121" s="19"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="28"/>
+      <c r="E121" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F121" s="41">
+        <v>45.0</v>
+      </c>
+      <c r="G121" s="42">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H121" s="43">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="122">
-      <c r="A122" s="6"/>
-      <c r="H122" s="6"/>
+      <c r="A122" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="28"/>
+      <c r="E122" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F122" s="44">
+        <v>8.0</v>
+      </c>
+      <c r="G122" s="45">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="H122" s="46">
+        <f t="shared" si="3"/>
+        <v>144</v>
+      </c>
     </row>
     <row r="123">
-      <c r="A123" s="6"/>
-      <c r="H123" s="6"/>
+      <c r="A123" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="28"/>
+      <c r="E123" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F123" s="41">
+        <v>65.0</v>
+      </c>
+      <c r="G123" s="42">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H123" s="43">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="124">
-      <c r="A124" s="6"/>
-      <c r="B124" s="6"/>
-      <c r="C124" s="6"/>
-      <c r="D124" s="6"/>
-      <c r="E124" s="6"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="6"/>
-      <c r="H124" s="6"/>
+      <c r="A124" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="28"/>
+      <c r="E124" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F124" s="44">
+        <v>90.0</v>
+      </c>
+      <c r="G124" s="45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H124" s="46">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="125">
-      <c r="A125" s="6"/>
-      <c r="B125" s="6"/>
-      <c r="C125" s="6"/>
-      <c r="D125" s="6"/>
-      <c r="E125" s="6"/>
-      <c r="F125" s="6"/>
-      <c r="G125" s="6"/>
-      <c r="H125" s="6"/>
+      <c r="A125" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B125" s="19"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="19"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="19"/>
+      <c r="G125" s="19"/>
+      <c r="H125" s="28"/>
     </row>
     <row r="126">
-      <c r="A126" s="6"/>
-      <c r="B126" s="6"/>
-      <c r="C126" s="6"/>
-      <c r="D126" s="6"/>
-      <c r="E126" s="6"/>
-      <c r="F126" s="6"/>
-      <c r="G126" s="6"/>
-      <c r="H126" s="6"/>
+      <c r="A126" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B126" s="19"/>
+      <c r="C126" s="19"/>
+      <c r="D126" s="28"/>
+      <c r="E126" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F126" s="44">
+        <v>3.0</v>
+      </c>
+      <c r="G126" s="45">
+        <f t="shared" ref="G126:G128" si="4">G104</f>
+        <v>222</v>
+      </c>
+      <c r="H126" s="46">
+        <f t="shared" ref="H126:H128" si="5">G126*F126</f>
+        <v>666</v>
+      </c>
     </row>
     <row r="127">
-      <c r="A127" s="6"/>
-      <c r="B127" s="6"/>
-      <c r="C127" s="6"/>
-      <c r="D127" s="6"/>
-      <c r="E127" s="6"/>
-      <c r="F127" s="6"/>
-      <c r="G127" s="6"/>
-      <c r="H127" s="6"/>
+      <c r="A127" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B127" s="19"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="28"/>
+      <c r="E127" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F127" s="41">
+        <v>30.0</v>
+      </c>
+      <c r="G127" s="42">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H127" s="43">
+        <f t="shared" si="5"/>
+        <v>270</v>
+      </c>
     </row>
     <row r="128">
-      <c r="A128" s="6"/>
-      <c r="B128" s="6"/>
-      <c r="C128" s="6"/>
-      <c r="D128" s="6"/>
-      <c r="E128" s="6"/>
-      <c r="F128" s="6"/>
-      <c r="G128" s="6"/>
-      <c r="H128" s="6"/>
+      <c r="A128" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B128" s="19"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="28"/>
+      <c r="E128" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F128" s="44">
+        <v>6.5</v>
+      </c>
+      <c r="G128" s="45">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="H128" s="46">
+        <f t="shared" si="5"/>
+        <v>409.5</v>
+      </c>
     </row>
     <row r="129">
-      <c r="A129" s="6"/>
-      <c r="B129" s="6"/>
-      <c r="C129" s="6"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="6"/>
-      <c r="F129" s="6"/>
-      <c r="G129" s="6"/>
-      <c r="H129" s="6"/>
+      <c r="A129" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="19"/>
+      <c r="G129" s="19"/>
+      <c r="H129" s="28"/>
     </row>
     <row r="130">
-      <c r="A130" s="6"/>
-      <c r="B130" s="6"/>
-      <c r="C130" s="6"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="6"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="6"/>
-      <c r="H130" s="6"/>
+      <c r="A130" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B130" s="19"/>
+      <c r="C130" s="19"/>
+      <c r="D130" s="28"/>
+      <c r="E130" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F130" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="G130" s="45">
+        <f>G108</f>
+        <v>100</v>
+      </c>
+      <c r="H130" s="46">
+        <f>G130*F130</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="131">
-      <c r="A131" s="6"/>
-      <c r="B131" s="6"/>
-      <c r="C131" s="6"/>
-      <c r="D131" s="6"/>
-      <c r="E131" s="6"/>
-      <c r="F131" s="6"/>
-      <c r="G131" s="6"/>
-      <c r="H131" s="6"/>
+      <c r="A131" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B131" s="19"/>
+      <c r="C131" s="19"/>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="19"/>
+      <c r="G131" s="28"/>
+      <c r="H131" s="47">
+        <f>sum(H117,H119:H124,H126:H128,H130)</f>
+        <v>5249.5</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="6"/>
@@ -2071,8 +2324,58 @@
       <c r="G164" s="6"/>
       <c r="H164" s="6"/>
     </row>
+    <row r="165">
+      <c r="A165" s="6"/>
+      <c r="B165" s="6"/>
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
+      <c r="E165" s="6"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="6"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="6"/>
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+      <c r="E166" s="6"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="6"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="6"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
+      <c r="E167" s="6"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="6"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="6"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
+      <c r="E168" s="6"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="66">
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A125:H125"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A130:D130"/>
     <mergeCell ref="B95:E95"/>
     <mergeCell ref="B96:G96"/>
     <mergeCell ref="A90:H94"/>
@@ -2121,6 +2424,14 @@
     <mergeCell ref="B108:E108"/>
     <mergeCell ref="B104:E104"/>
     <mergeCell ref="B105:E105"/>
+    <mergeCell ref="A110:H113"/>
+    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A116:H116"/>
+    <mergeCell ref="A118:H118"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="A129:H129"/>
+    <mergeCell ref="A131:G131"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>